<commit_message>
added target for total referrals given and honored
</commit_message>
<xml_diff>
--- a/forms/contact/household-create.xlsx
+++ b/forms/contact/household-create.xlsx
@@ -763,35 +763,7 @@
     <t xml:space="preserve">n_hh_age</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;h4 style="text-align:center;"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">${person_age_years} ${dob_iso}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/h4&gt;</t>
-    </r>
+    <t xml:space="preserve">&lt;h4 style="text-align:center;"&gt;${person_age_years} ${dob_iso}&lt;/h4&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">n_submit</t>
@@ -1013,7 +985,7 @@
     <t xml:space="preserve">New Household</t>
   </si>
   <si>
-    <t xml:space="preserve">contact:household:create</t>
+    <t xml:space="preserve">household_create</t>
   </si>
   <si>
     <t xml:space="preserve">2020-01-27</t>
@@ -1058,7 +1030,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1130,12 +1102,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -1376,7 +1342,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1481,7 +1447,7 @@
       <selection pane="bottomLeft" activeCell="C105" activeCellId="0" sqref="C105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.43"/>
@@ -6363,7 +6329,7 @@
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10"/>
@@ -8309,7 +8275,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.71"/>
@@ -9398,7 +9364,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="1.86"/>

</xml_diff>

<commit_message>
better household creation form
</commit_message>
<xml_diff>
--- a/forms/contact/household-create.xlsx
+++ b/forms/contact/household-create.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="340">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -418,12 +418,30 @@
     <t xml:space="preserve">Does the household have hand washing facility?</t>
   </si>
   <si>
+    <t xml:space="preserve">handwashings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p style = "color:red; font-weight:bold"&gt;Teach the household on the importance of hand washing facility in the household.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${handwashing} = ‘no’</t>
+  </si>
+  <si>
     <t xml:space="preserve">latrine</t>
   </si>
   <si>
     <t xml:space="preserve">Does the household have a functional latrine that is in use?</t>
   </si>
   <si>
+    <t xml:space="preserve">latrines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p style = "color:red; font-weight:bold"&gt;Encourage the household to get a functional latrine.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${latrine} =  ‘no’</t>
+  </si>
+  <si>
     <t xml:space="preserve">hidden</t>
   </si>
   <si>
@@ -658,31 +676,7 @@
     <t xml:space="preserve">UMRI: ${person_age_years} ${dob_iso}</t>
   </si>
   <si>
-    <t xml:space="preserve">tel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nambari ya simu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${person_age_years} &gt;=10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please make sure the number is not already in use by another person and is in the format 07XX XXX XXX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use the following format: 07XX XXX XXX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">secondary_phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary Phone Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nambari ya Simu ya Sekondari</t>
+    <t xml:space="preserve">secs_phone</t>
   </si>
   <si>
     <t xml:space="preserve">select_one family_designation</t>
@@ -760,10 +754,64 @@
     <t xml:space="preserve">&lt;h4 style="text-align:center;"&gt;${pri_phone}&lt;/h4&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">n_hh_age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h4 style="text-align:center;"&gt;${person_age_years} ${dob_iso}&lt;/h4&gt;</t>
+    <t xml:space="preserve">findings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Household Data &lt;i class="fa fa-warning" aria-hidden="true"&gt;&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${water}  =  ‘yes’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">watertreatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They treat water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${treatment} =  ‘yes’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nowatertreatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They do not treat water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${treatment} =  ‘no’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">handfacility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hand washing Facility is available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${handwashing} =  ‘yes’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nohandfacility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No hand washing facility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${handwashing} =  ‘no’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latriness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They have a functional latrine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${latrine} =  ‘yes’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nolatrine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No functional latrine</t>
   </si>
   <si>
     <t xml:space="preserve">n_submit</t>
@@ -1022,12 +1070,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1096,6 +1143,19 @@
     <font>
       <sz val="10"/>
       <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
@@ -1214,7 +1274,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1299,11 +1359,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1335,11 +1403,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1436,15 +1504,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB1048576"/>
+  <dimension ref="A1:AB1004"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C105" activeCellId="0" sqref="C105"/>
+      <selection pane="bottomLeft" activeCell="C112" activeCellId="0" sqref="C112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.43"/>
@@ -3173,24 +3241,24 @@
       <c r="AB45" s="7"/>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B46" s="7" t="s">
+      <c r="A46" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D46" s="7"/>
-      <c r="E46" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F46" s="16"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="10" t="s">
+        <v>126</v>
+      </c>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
-      <c r="J46" s="10"/>
+      <c r="J46" s="7"/>
       <c r="K46" s="7"/>
       <c r="L46" s="7"/>
       <c r="M46" s="7"/>
@@ -3211,44 +3279,58 @@
       <c r="AB46" s="7"/>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="5"/>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5"/>
-      <c r="W47" s="5"/>
-      <c r="X47" s="5"/>
-      <c r="Y47" s="5"/>
-      <c r="Z47" s="5"/>
-      <c r="AA47" s="5"/>
-      <c r="AB47" s="5"/>
+      <c r="A47" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F47" s="16"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="7"/>
+      <c r="S47" s="7"/>
+      <c r="T47" s="7"/>
+      <c r="U47" s="7"/>
+      <c r="V47" s="7"/>
+      <c r="W47" s="7"/>
+      <c r="X47" s="7"/>
+      <c r="Y47" s="7"/>
+      <c r="Z47" s="7"/>
+      <c r="AA47" s="7"/>
+      <c r="AB47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
+      <c r="A48" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>130</v>
+      </c>
       <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
@@ -3274,20 +3356,14 @@
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>106</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
-      <c r="G49" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="G49" s="5"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
@@ -3310,88 +3386,80 @@
       <c r="AA49" s="5"/>
       <c r="AB49" s="5"/>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
-      <c r="J50" s="17"/>
-      <c r="K50" s="17"/>
-      <c r="L50" s="17"/>
-      <c r="M50" s="17"/>
-      <c r="N50" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="O50" s="17"/>
-      <c r="P50" s="17"/>
-      <c r="Q50" s="17"/>
-      <c r="R50" s="17"/>
-      <c r="S50" s="17"/>
-      <c r="T50" s="17"/>
-      <c r="U50" s="17"/>
-      <c r="V50" s="17"/>
-      <c r="W50" s="17"/>
-      <c r="X50" s="17"/>
-      <c r="Y50" s="17"/>
-      <c r="Z50" s="17"/>
-      <c r="AA50" s="17"/>
-      <c r="AB50" s="17"/>
-    </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="17"/>
-      <c r="J51" s="17"/>
-      <c r="K51" s="17"/>
-      <c r="L51" s="17"/>
-      <c r="M51" s="17"/>
-      <c r="N51" s="17" t="s">
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+      <c r="S50" s="7"/>
+      <c r="T50" s="7"/>
+      <c r="U50" s="7"/>
+      <c r="V50" s="7"/>
+      <c r="W50" s="7"/>
+      <c r="X50" s="7"/>
+      <c r="Y50" s="7"/>
+      <c r="Z50" s="7"/>
+      <c r="AA50" s="7"/>
+      <c r="AB50" s="7"/>
+    </row>
+    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="O51" s="17"/>
-      <c r="P51" s="17"/>
-      <c r="Q51" s="17"/>
-      <c r="R51" s="17"/>
-      <c r="S51" s="17"/>
-      <c r="T51" s="17"/>
-      <c r="U51" s="17"/>
-      <c r="V51" s="17"/>
-      <c r="W51" s="17"/>
-      <c r="X51" s="17"/>
-      <c r="Y51" s="17"/>
-      <c r="Z51" s="17"/>
-      <c r="AA51" s="17"/>
-      <c r="AB51" s="17"/>
-    </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C51" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="5"/>
+      <c r="S51" s="5"/>
+      <c r="T51" s="5"/>
+      <c r="U51" s="5"/>
+      <c r="V51" s="5"/>
+      <c r="W51" s="5"/>
+      <c r="X51" s="5"/>
+      <c r="Y51" s="5"/>
+      <c r="Z51" s="5"/>
+      <c r="AA51" s="5"/>
+      <c r="AB51" s="5"/>
+    </row>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="17" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>17</v>
@@ -3407,7 +3475,7 @@
       <c r="L52" s="17"/>
       <c r="M52" s="17"/>
       <c r="N52" s="17" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="O52" s="17"/>
       <c r="P52" s="17"/>
@@ -3424,27 +3492,29 @@
       <c r="AA52" s="17"/>
       <c r="AB52" s="17"/>
     </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="B53" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
-      <c r="I53" s="19"/>
-      <c r="J53" s="19"/>
-      <c r="K53" s="19" t="s">
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="17" t="s">
         <v>132</v>
       </c>
+      <c r="B53" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
       <c r="L53" s="17"/>
       <c r="M53" s="17"/>
-      <c r="N53" s="17"/>
+      <c r="N53" s="17" t="s">
+        <v>28</v>
+      </c>
       <c r="O53" s="17"/>
       <c r="P53" s="17"/>
       <c r="Q53" s="17"/>
@@ -3462,13 +3532,13 @@
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="17" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>134</v>
+        <v>17</v>
       </c>
       <c r="D54" s="17"/>
       <c r="E54" s="17"/>
@@ -3477,12 +3547,12 @@
       <c r="H54" s="17"/>
       <c r="I54" s="17"/>
       <c r="J54" s="17"/>
-      <c r="K54" s="18" t="s">
-        <v>135</v>
-      </c>
+      <c r="K54" s="17"/>
       <c r="L54" s="17"/>
       <c r="M54" s="17"/>
-      <c r="N54" s="17"/>
+      <c r="N54" s="17" t="s">
+        <v>136</v>
+      </c>
       <c r="O54" s="17"/>
       <c r="P54" s="17"/>
       <c r="Q54" s="17"/>
@@ -3499,25 +3569,21 @@
       <c r="AB54" s="17"/>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B55" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="D55" s="17" t="s">
+      <c r="B55" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="17"/>
-      <c r="J55" s="17"/>
-      <c r="K55" s="17" t="s">
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19" t="s">
         <v>138</v>
       </c>
       <c r="L55" s="17"/>
@@ -3545,7 +3611,9 @@
       <c r="B56" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="C56" s="17"/>
+      <c r="C56" s="17" t="s">
+        <v>140</v>
+      </c>
       <c r="D56" s="17"/>
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
@@ -3553,8 +3621,8 @@
       <c r="H56" s="17"/>
       <c r="I56" s="17"/>
       <c r="J56" s="17"/>
-      <c r="K56" s="17" t="s">
-        <v>140</v>
+      <c r="K56" s="18" t="s">
+        <v>141</v>
       </c>
       <c r="L56" s="17"/>
       <c r="M56" s="17"/>
@@ -3576,10 +3644,10 @@
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="17" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>141</v>
+        <v>1</v>
       </c>
       <c r="C57" s="17" t="s">
         <v>142</v>
@@ -3593,7 +3661,9 @@
       <c r="H57" s="17"/>
       <c r="I57" s="17"/>
       <c r="J57" s="17"/>
-      <c r="K57" s="17"/>
+      <c r="K57" s="17" t="s">
+        <v>144</v>
+      </c>
       <c r="L57" s="17"/>
       <c r="M57" s="17"/>
       <c r="N57" s="17"/>
@@ -3613,185 +3683,175 @@
       <c r="AB57" s="17"/>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="L58" s="17"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="17"/>
+      <c r="O58" s="17"/>
+      <c r="P58" s="17"/>
+      <c r="Q58" s="17"/>
+      <c r="R58" s="17"/>
+      <c r="S58" s="17"/>
+      <c r="T58" s="17"/>
+      <c r="U58" s="17"/>
+      <c r="V58" s="17"/>
+      <c r="W58" s="17"/>
+      <c r="X58" s="17"/>
+      <c r="Y58" s="17"/>
+      <c r="Z58" s="17"/>
+      <c r="AA58" s="17"/>
+      <c r="AB58" s="17"/>
+    </row>
+    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="17"/>
+      <c r="P59" s="17"/>
+      <c r="Q59" s="17"/>
+      <c r="R59" s="17"/>
+      <c r="S59" s="17"/>
+      <c r="T59" s="17"/>
+      <c r="U59" s="17"/>
+      <c r="V59" s="17"/>
+      <c r="W59" s="17"/>
+      <c r="X59" s="17"/>
+      <c r="Y59" s="17"/>
+      <c r="Z59" s="17"/>
+      <c r="AA59" s="17"/>
+      <c r="AB59" s="17"/>
+    </row>
+    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
-      <c r="J58" s="5"/>
-      <c r="K58" s="5"/>
-      <c r="L58" s="5"/>
-      <c r="M58" s="5"/>
-      <c r="N58" s="5"/>
-      <c r="O58" s="5"/>
-      <c r="P58" s="5"/>
-      <c r="Q58" s="5"/>
-      <c r="R58" s="5"/>
-      <c r="S58" s="5"/>
-      <c r="T58" s="5"/>
-      <c r="U58" s="5"/>
-      <c r="V58" s="5"/>
-      <c r="W58" s="5"/>
-      <c r="X58" s="5"/>
-      <c r="Y58" s="5"/>
-      <c r="Z58" s="5"/>
-      <c r="AA58" s="5"/>
-      <c r="AB58" s="5"/>
-    </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="s">
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+      <c r="O60" s="5"/>
+      <c r="P60" s="5"/>
+      <c r="Q60" s="5"/>
+      <c r="R60" s="5"/>
+      <c r="S60" s="5"/>
+      <c r="T60" s="5"/>
+      <c r="U60" s="5"/>
+      <c r="V60" s="5"/>
+      <c r="W60" s="5"/>
+      <c r="X60" s="5"/>
+      <c r="Y60" s="5"/>
+      <c r="Z60" s="5"/>
+      <c r="AA60" s="5"/>
+      <c r="AB60" s="5"/>
+    </row>
+    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5" t="s">
+      <c r="B61" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
-      <c r="J59" s="5"/>
-      <c r="K59" s="5"/>
-      <c r="L59" s="5"/>
-      <c r="M59" s="5"/>
-      <c r="N59" s="5"/>
-      <c r="O59" s="5"/>
-      <c r="P59" s="5"/>
-      <c r="Q59" s="5"/>
-      <c r="R59" s="5"/>
-      <c r="S59" s="5"/>
-      <c r="T59" s="5"/>
-      <c r="U59" s="5"/>
-      <c r="V59" s="5"/>
-      <c r="W59" s="5"/>
-      <c r="X59" s="5"/>
-      <c r="Y59" s="5"/>
-      <c r="Z59" s="5"/>
-      <c r="AA59" s="5"/>
-      <c r="AB59" s="5"/>
-    </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17"/>
-      <c r="J60" s="17"/>
-      <c r="K60" s="17"/>
-      <c r="L60" s="17"/>
-      <c r="M60" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="N60" s="17"/>
-      <c r="O60" s="17"/>
-      <c r="P60" s="17"/>
-      <c r="Q60" s="17"/>
-      <c r="R60" s="17"/>
-      <c r="S60" s="17"/>
-      <c r="T60" s="17"/>
-      <c r="U60" s="17"/>
-      <c r="V60" s="17"/>
-      <c r="W60" s="17"/>
-      <c r="X60" s="17"/>
-      <c r="Y60" s="17"/>
-      <c r="Z60" s="17"/>
-      <c r="AA60" s="17"/>
-      <c r="AB60" s="17"/>
-    </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D61" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="E61" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F61" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="G61" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
-      <c r="J61" s="17"/>
-      <c r="K61" s="17"/>
-      <c r="L61" s="17"/>
-      <c r="M61" s="17"/>
-      <c r="N61" s="17"/>
-      <c r="O61" s="17"/>
-      <c r="P61" s="17"/>
-      <c r="Q61" s="17"/>
-      <c r="R61" s="17"/>
-      <c r="S61" s="17"/>
-      <c r="T61" s="17"/>
-      <c r="U61" s="17"/>
-      <c r="V61" s="17"/>
-      <c r="W61" s="17"/>
-      <c r="X61" s="17"/>
-      <c r="Y61" s="17"/>
-      <c r="Z61" s="17"/>
-      <c r="AA61" s="17"/>
-      <c r="AB61" s="17"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="5"/>
+      <c r="O61" s="5"/>
+      <c r="P61" s="5"/>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="5"/>
+      <c r="S61" s="5"/>
+      <c r="T61" s="5"/>
+      <c r="U61" s="5"/>
+      <c r="V61" s="5"/>
+      <c r="W61" s="5"/>
+      <c r="X61" s="5"/>
+      <c r="Y61" s="5"/>
+      <c r="Z61" s="5"/>
+      <c r="AA61" s="5"/>
+      <c r="AB61" s="5"/>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="17" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E62" s="17"/>
-      <c r="F62" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="G62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17" t="s">
+        <v>68</v>
+      </c>
       <c r="H62" s="17"/>
       <c r="I62" s="17"/>
       <c r="J62" s="17"/>
       <c r="K62" s="17"/>
       <c r="L62" s="17"/>
-      <c r="M62" s="17"/>
+      <c r="M62" s="17" t="s">
+        <v>155</v>
+      </c>
       <c r="N62" s="17"/>
       <c r="O62" s="17"/>
       <c r="P62" s="17"/>
@@ -3809,92 +3869,96 @@
       <c r="AB62" s="17"/>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
-      <c r="L63" s="5"/>
-      <c r="M63" s="5"/>
-      <c r="N63" s="5"/>
-      <c r="O63" s="5"/>
-      <c r="P63" s="5"/>
-      <c r="Q63" s="5"/>
-      <c r="R63" s="5"/>
-      <c r="S63" s="5"/>
-      <c r="T63" s="5"/>
-      <c r="U63" s="5"/>
-      <c r="V63" s="5"/>
-      <c r="W63" s="5"/>
-      <c r="X63" s="5"/>
-      <c r="Y63" s="5"/>
-      <c r="Z63" s="5"/>
-      <c r="AA63" s="5"/>
-      <c r="AB63" s="5"/>
+      <c r="A63" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D63" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="E63" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G63" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="17"/>
+      <c r="O63" s="17"/>
+      <c r="P63" s="17"/>
+      <c r="Q63" s="17"/>
+      <c r="R63" s="17"/>
+      <c r="S63" s="17"/>
+      <c r="T63" s="17"/>
+      <c r="U63" s="17"/>
+      <c r="V63" s="17"/>
+      <c r="W63" s="17"/>
+      <c r="X63" s="17"/>
+      <c r="Y63" s="17"/>
+      <c r="Z63" s="17"/>
+      <c r="AA63" s="17"/>
+      <c r="AB63" s="17"/>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5" t="s">
+      <c r="A64" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B64" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="G64" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
-      <c r="L64" s="5"/>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5"/>
-      <c r="O64" s="5"/>
-      <c r="P64" s="5"/>
-      <c r="Q64" s="5"/>
-      <c r="R64" s="5"/>
-      <c r="S64" s="5"/>
-      <c r="T64" s="5"/>
-      <c r="U64" s="5"/>
-      <c r="V64" s="5"/>
-      <c r="W64" s="5"/>
-      <c r="X64" s="5"/>
-      <c r="Y64" s="5"/>
-      <c r="Z64" s="5"/>
-      <c r="AA64" s="5"/>
-      <c r="AB64" s="5"/>
+      <c r="C64" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+      <c r="J64" s="17"/>
+      <c r="K64" s="17"/>
+      <c r="L64" s="17"/>
+      <c r="M64" s="17"/>
+      <c r="N64" s="17"/>
+      <c r="O64" s="17"/>
+      <c r="P64" s="17"/>
+      <c r="Q64" s="17"/>
+      <c r="R64" s="17"/>
+      <c r="S64" s="17"/>
+      <c r="T64" s="17"/>
+      <c r="U64" s="17"/>
+      <c r="V64" s="17"/>
+      <c r="W64" s="17"/>
+      <c r="X64" s="17"/>
+      <c r="Y64" s="17"/>
+      <c r="Z64" s="17"/>
+      <c r="AA64" s="17"/>
+      <c r="AB64" s="17"/>
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>164</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
@@ -3920,89 +3984,95 @@
       <c r="AA65" s="5"/>
       <c r="AB65" s="5"/>
     </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B66" s="17" t="s">
+    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C66" s="17" t="s">
+      <c r="C66" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="17"/>
-      <c r="J66" s="17"/>
-      <c r="K66" s="17"/>
-      <c r="L66" s="17"/>
-      <c r="M66" s="17"/>
-      <c r="N66" s="17"/>
-      <c r="O66" s="17"/>
-      <c r="P66" s="17"/>
-      <c r="Q66" s="17"/>
-      <c r="R66" s="17"/>
-      <c r="S66" s="17"/>
-      <c r="T66" s="17"/>
-      <c r="U66" s="17"/>
-      <c r="V66" s="17"/>
-      <c r="W66" s="17"/>
-      <c r="X66" s="17"/>
-      <c r="Y66" s="17"/>
-      <c r="Z66" s="17"/>
-      <c r="AA66" s="17"/>
-      <c r="AB66" s="17"/>
-    </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="17"/>
-      <c r="J67" s="17"/>
-      <c r="K67" s="17"/>
-      <c r="L67" s="17"/>
-      <c r="M67" s="17"/>
-      <c r="N67" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="O67" s="17"/>
-      <c r="P67" s="17"/>
-      <c r="Q67" s="17"/>
-      <c r="R67" s="17"/>
-      <c r="S67" s="17"/>
-      <c r="T67" s="17"/>
-      <c r="U67" s="17"/>
-      <c r="V67" s="17"/>
-      <c r="W67" s="17"/>
-      <c r="X67" s="17"/>
-      <c r="Y67" s="17"/>
-      <c r="Z67" s="17"/>
-      <c r="AA67" s="17"/>
-      <c r="AB67" s="17"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="5"/>
+      <c r="O66" s="5"/>
+      <c r="P66" s="5"/>
+      <c r="Q66" s="5"/>
+      <c r="R66" s="5"/>
+      <c r="S66" s="5"/>
+      <c r="T66" s="5"/>
+      <c r="U66" s="5"/>
+      <c r="V66" s="5"/>
+      <c r="W66" s="5"/>
+      <c r="X66" s="5"/>
+      <c r="Y66" s="5"/>
+      <c r="Z66" s="5"/>
+      <c r="AA66" s="5"/>
+      <c r="AB66" s="5"/>
+    </row>
+    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+      <c r="O67" s="5"/>
+      <c r="P67" s="5"/>
+      <c r="Q67" s="5"/>
+      <c r="R67" s="5"/>
+      <c r="S67" s="5"/>
+      <c r="T67" s="5"/>
+      <c r="U67" s="5"/>
+      <c r="V67" s="5"/>
+      <c r="W67" s="5"/>
+      <c r="X67" s="5"/>
+      <c r="Y67" s="5"/>
+      <c r="Z67" s="5"/>
+      <c r="AA67" s="5"/>
+      <c r="AB67" s="5"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="17" t="s">
-        <v>126</v>
+        <v>37</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>129</v>
+        <v>171</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
       <c r="D68" s="17"/>
       <c r="E68" s="17"/>
@@ -4013,12 +4083,8 @@
       <c r="J68" s="17"/>
       <c r="K68" s="17"/>
       <c r="L68" s="17"/>
-      <c r="M68" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="N68" s="17" t="s">
-        <v>130</v>
-      </c>
+      <c r="M68" s="17"/>
+      <c r="N68" s="17"/>
       <c r="O68" s="17"/>
       <c r="P68" s="17"/>
       <c r="Q68" s="17"/>
@@ -4036,10 +4102,10 @@
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="17" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="C69" s="17" t="s">
         <v>17</v>
@@ -4053,11 +4119,9 @@
       <c r="J69" s="17"/>
       <c r="K69" s="17"/>
       <c r="L69" s="17"/>
-      <c r="M69" s="17" t="s">
-        <v>167</v>
-      </c>
+      <c r="M69" s="17"/>
       <c r="N69" s="17" t="s">
-        <v>128</v>
+        <v>28</v>
       </c>
       <c r="O69" s="17"/>
       <c r="P69" s="17"/>
@@ -4076,20 +4140,16 @@
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="17" t="s">
-        <v>20</v>
+        <v>132</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="D70" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E70" s="17" t="s">
-        <v>36</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
       <c r="F70" s="17"/>
       <c r="G70" s="17"/>
       <c r="H70" s="17"/>
@@ -4097,10 +4157,12 @@
       <c r="J70" s="17"/>
       <c r="K70" s="17"/>
       <c r="L70" s="17"/>
-      <c r="M70" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="N70" s="17"/>
+      <c r="M70" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="N70" s="17" t="s">
+        <v>136</v>
+      </c>
       <c r="O70" s="17"/>
       <c r="P70" s="17"/>
       <c r="Q70" s="17"/>
@@ -4118,10 +4180,10 @@
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="17" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="C71" s="17" t="s">
         <v>17</v>
@@ -4133,12 +4195,14 @@
       <c r="H71" s="17"/>
       <c r="I71" s="17"/>
       <c r="J71" s="17"/>
-      <c r="K71" s="17" t="s">
-        <v>169</v>
-      </c>
+      <c r="K71" s="17"/>
       <c r="L71" s="17"/>
-      <c r="M71" s="17"/>
-      <c r="N71" s="17"/>
+      <c r="M71" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="N71" s="17" t="s">
+        <v>134</v>
+      </c>
       <c r="O71" s="17"/>
       <c r="P71" s="17"/>
       <c r="Q71" s="17"/>
@@ -4154,30 +4218,32 @@
       <c r="AA71" s="17"/>
       <c r="AB71" s="17"/>
     </row>
-    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>170</v>
+        <v>1</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="D72" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="E72" s="17"/>
+        <v>143</v>
+      </c>
+      <c r="E72" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="F72" s="17"/>
-      <c r="G72" s="17" t="s">
-        <v>126</v>
-      </c>
+      <c r="G72" s="17"/>
       <c r="H72" s="17"/>
       <c r="I72" s="17"/>
       <c r="J72" s="17"/>
       <c r="K72" s="17"/>
       <c r="L72" s="17"/>
-      <c r="M72" s="17"/>
+      <c r="M72" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="N72" s="17"/>
       <c r="O72" s="17"/>
       <c r="P72" s="17"/>
@@ -4194,30 +4260,26 @@
       <c r="AA72" s="17"/>
       <c r="AB72" s="17"/>
     </row>
-    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="17" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D73" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E73" s="17" t="s">
-        <v>36</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
       <c r="F73" s="17"/>
-      <c r="G73" s="17" t="s">
-        <v>68</v>
-      </c>
+      <c r="G73" s="17"/>
       <c r="H73" s="17"/>
       <c r="I73" s="17"/>
       <c r="J73" s="17"/>
-      <c r="K73" s="17"/>
+      <c r="K73" s="17" t="s">
+        <v>175</v>
+      </c>
       <c r="L73" s="17"/>
       <c r="M73" s="17"/>
       <c r="N73" s="17"/>
@@ -4238,26 +4300,26 @@
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="17" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>131</v>
+        <v>176</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>74</v>
+        <v>177</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>75</v>
+        <v>178</v>
       </c>
       <c r="E74" s="17"/>
       <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
+      <c r="G74" s="17" t="s">
+        <v>132</v>
+      </c>
       <c r="H74" s="17"/>
       <c r="I74" s="17"/>
       <c r="J74" s="17"/>
-      <c r="K74" s="17" t="s">
-        <v>173</v>
-      </c>
+      <c r="K74" s="17"/>
       <c r="L74" s="17"/>
       <c r="M74" s="17"/>
       <c r="N74" s="17"/>
@@ -4278,16 +4340,16 @@
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="17" t="s">
-        <v>174</v>
+        <v>64</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>175</v>
+        <v>139</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>176</v>
+        <v>66</v>
       </c>
       <c r="D75" s="17" t="s">
-        <v>177</v>
+        <v>67</v>
       </c>
       <c r="E75" s="17" t="s">
         <v>36</v>
@@ -4320,30 +4382,26 @@
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="17" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>178</v>
+        <v>74</v>
       </c>
       <c r="D76" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="E76" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F76" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="G76" s="17" t="s">
-        <v>68</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E76" s="17"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="17"/>
       <c r="H76" s="17"/>
       <c r="I76" s="17"/>
       <c r="J76" s="17"/>
-      <c r="K76" s="17"/>
+      <c r="K76" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="L76" s="17"/>
       <c r="M76" s="17"/>
       <c r="N76" s="17"/>
@@ -4364,31 +4422,27 @@
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="17" t="s">
-        <v>72</v>
+        <v>180</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>73</v>
+        <v>181</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>75</v>
+        <v>183</v>
       </c>
       <c r="E77" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F77" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="G77" s="17"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="17" t="s">
+        <v>68</v>
+      </c>
       <c r="H77" s="17"/>
-      <c r="I77" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="J77" s="17" t="s">
-        <v>183</v>
-      </c>
+      <c r="I77" s="17"/>
+      <c r="J77" s="17"/>
       <c r="K77" s="17"/>
       <c r="L77" s="17"/>
       <c r="M77" s="17"/>
@@ -4410,36 +4464,32 @@
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="17" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="B78" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C78" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="C78" s="17" t="s">
-        <v>81</v>
-      </c>
       <c r="D78" s="17" t="s">
-        <v>82</v>
+        <v>185</v>
       </c>
       <c r="E78" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F78" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="G78" s="17"/>
+        <v>186</v>
+      </c>
+      <c r="G78" s="17" t="s">
+        <v>68</v>
+      </c>
       <c r="H78" s="17"/>
-      <c r="I78" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="J78" s="17" t="s">
-        <v>183</v>
-      </c>
+      <c r="I78" s="17"/>
+      <c r="J78" s="17"/>
       <c r="K78" s="17"/>
       <c r="L78" s="17"/>
-      <c r="M78" s="17" t="s">
-        <v>187</v>
-      </c>
+      <c r="M78" s="17"/>
       <c r="N78" s="17"/>
       <c r="O78" s="17"/>
       <c r="P78" s="17"/>
@@ -4458,29 +4508,35 @@
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="17" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>188</v>
+        <v>73</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D79" s="17"/>
-      <c r="E79" s="17"/>
-      <c r="F79" s="17"/>
+        <v>74</v>
+      </c>
+      <c r="D79" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E79" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F79" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="G79" s="17"/>
       <c r="H79" s="17"/>
-      <c r="I79" s="17"/>
-      <c r="J79" s="17"/>
-      <c r="K79" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="I79" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="J79" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="K79" s="17"/>
       <c r="L79" s="17"/>
       <c r="M79" s="17"/>
-      <c r="N79" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="N79" s="17"/>
       <c r="O79" s="17"/>
       <c r="P79" s="17"/>
       <c r="Q79" s="17"/>
@@ -4498,26 +4554,36 @@
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="17" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
+        <v>81</v>
+      </c>
+      <c r="D80" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E80" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F80" s="17" t="s">
+        <v>191</v>
+      </c>
       <c r="G80" s="17"/>
       <c r="H80" s="17"/>
-      <c r="I80" s="17"/>
-      <c r="J80" s="17"/>
-      <c r="K80" s="17" t="s">
-        <v>190</v>
-      </c>
+      <c r="I80" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="J80" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="K80" s="17"/>
       <c r="L80" s="17"/>
-      <c r="M80" s="17"/>
+      <c r="M80" s="17" t="s">
+        <v>193</v>
+      </c>
       <c r="N80" s="17"/>
       <c r="O80" s="17"/>
       <c r="P80" s="17"/>
@@ -4539,7 +4605,7 @@
         <v>85</v>
       </c>
       <c r="B81" s="17" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C81" s="17" t="s">
         <v>17</v>
@@ -4551,12 +4617,14 @@
       <c r="H81" s="17"/>
       <c r="I81" s="17"/>
       <c r="J81" s="17"/>
-      <c r="K81" s="17" t="s">
-        <v>192</v>
+      <c r="K81" s="17" t="n">
+        <v>0</v>
       </c>
       <c r="L81" s="17"/>
       <c r="M81" s="17"/>
-      <c r="N81" s="17"/>
+      <c r="N81" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="O81" s="17"/>
       <c r="P81" s="17"/>
       <c r="Q81" s="17"/>
@@ -4577,7 +4645,7 @@
         <v>85</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C82" s="17" t="s">
         <v>17</v>
@@ -4590,7 +4658,7 @@
       <c r="I82" s="17"/>
       <c r="J82" s="17"/>
       <c r="K82" s="17" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="L82" s="17"/>
       <c r="M82" s="17"/>
@@ -4615,7 +4683,7 @@
         <v>85</v>
       </c>
       <c r="B83" s="17" t="s">
-        <v>86</v>
+        <v>197</v>
       </c>
       <c r="C83" s="17" t="s">
         <v>17</v>
@@ -4628,7 +4696,7 @@
       <c r="I83" s="17"/>
       <c r="J83" s="17"/>
       <c r="K83" s="17" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="L83" s="17"/>
       <c r="M83" s="17"/>
@@ -4653,7 +4721,7 @@
         <v>85</v>
       </c>
       <c r="B84" s="17" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C84" s="17" t="s">
         <v>17</v>
@@ -4666,7 +4734,7 @@
       <c r="I84" s="17"/>
       <c r="J84" s="17"/>
       <c r="K84" s="17" t="s">
-        <v>89</v>
+        <v>200</v>
       </c>
       <c r="L84" s="17"/>
       <c r="M84" s="17"/>
@@ -4691,7 +4759,7 @@
         <v>85</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>197</v>
+        <v>86</v>
       </c>
       <c r="C85" s="17" t="s">
         <v>17</v>
@@ -4704,7 +4772,7 @@
       <c r="I85" s="17"/>
       <c r="J85" s="17"/>
       <c r="K85" s="17" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="L85" s="17"/>
       <c r="M85" s="17"/>
@@ -4729,7 +4797,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C86" s="17" t="s">
         <v>17</v>
@@ -4742,7 +4810,7 @@
       <c r="I86" s="17"/>
       <c r="J86" s="17"/>
       <c r="K86" s="17" t="s">
-        <v>200</v>
+        <v>89</v>
       </c>
       <c r="L86" s="17"/>
       <c r="M86" s="17"/>
@@ -4764,27 +4832,24 @@
     </row>
     <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="17" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="B87" s="17" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="D87" s="17" t="s">
-        <v>203</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D87" s="17"/>
       <c r="E87" s="17"/>
-      <c r="F87" s="21" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="F87" s="17"/>
       <c r="G87" s="17"/>
       <c r="H87" s="17"/>
       <c r="I87" s="17"/>
       <c r="J87" s="17"/>
-      <c r="K87" s="17"/>
+      <c r="K87" s="17" t="s">
+        <v>204</v>
+      </c>
       <c r="L87" s="17"/>
       <c r="M87" s="17"/>
       <c r="N87" s="17"/>
@@ -4805,35 +4870,26 @@
     </row>
     <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="17" t="s">
-        <v>204</v>
+        <v>85</v>
       </c>
       <c r="B88" s="17" t="s">
-        <v>139</v>
+        <v>205</v>
       </c>
       <c r="C88" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="D88" s="17" t="s">
-        <v>206</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D88" s="17"/>
       <c r="E88" s="17"/>
-      <c r="F88" s="17" t="s">
-        <v>207</v>
-      </c>
+      <c r="F88" s="17"/>
       <c r="G88" s="17"/>
       <c r="H88" s="17"/>
-      <c r="I88" s="19" t="n">
-        <f aca="false">1</f>
-        <v>1</v>
-      </c>
-      <c r="J88" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="K88" s="17"/>
+      <c r="I88" s="17"/>
+      <c r="J88" s="17"/>
+      <c r="K88" s="17" t="s">
+        <v>206</v>
+      </c>
       <c r="L88" s="17"/>
-      <c r="M88" s="17" t="s">
-        <v>209</v>
-      </c>
+      <c r="M88" s="17"/>
       <c r="N88" s="17"/>
       <c r="O88" s="17"/>
       <c r="P88" s="17"/>
@@ -4852,35 +4908,29 @@
     </row>
     <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="17" t="s">
-        <v>204</v>
+        <v>37</v>
       </c>
       <c r="B89" s="17" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D89" s="17" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E89" s="17"/>
-      <c r="F89" s="17" t="s">
-        <v>207</v>
+      <c r="F89" s="21" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="G89" s="17"/>
       <c r="H89" s="17"/>
-      <c r="I89" s="19" t="n">
-        <f aca="false">1</f>
-        <v>1</v>
-      </c>
-      <c r="J89" s="17" t="s">
-        <v>208</v>
-      </c>
+      <c r="I89" s="17"/>
+      <c r="J89" s="17"/>
       <c r="K89" s="17"/>
       <c r="L89" s="17"/>
-      <c r="M89" s="17" t="s">
-        <v>209</v>
-      </c>
+      <c r="M89" s="17"/>
       <c r="N89" s="17"/>
       <c r="O89" s="17"/>
       <c r="P89" s="17"/>
@@ -4899,25 +4949,27 @@
     </row>
     <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="17" t="s">
-        <v>213</v>
+        <v>56</v>
       </c>
       <c r="B90" s="17" t="s">
-        <v>214</v>
+        <v>145</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>215</v>
+        <v>91</v>
       </c>
       <c r="D90" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="E90" s="17" t="s">
-        <v>36</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E90" s="17"/>
       <c r="F90" s="17"/>
       <c r="G90" s="17"/>
       <c r="H90" s="17"/>
-      <c r="I90" s="17"/>
-      <c r="J90" s="17"/>
+      <c r="I90" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="J90" s="16" t="s">
+        <v>94</v>
+      </c>
       <c r="K90" s="17"/>
       <c r="L90" s="17"/>
       <c r="M90" s="17"/>
@@ -4942,24 +4994,24 @@
         <v>56</v>
       </c>
       <c r="B91" s="17" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>218</v>
+        <v>96</v>
       </c>
       <c r="D91" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="E91" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F91" s="17" t="s">
-        <v>220</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E91" s="17"/>
+      <c r="F91" s="17"/>
       <c r="G91" s="17"/>
       <c r="H91" s="17"/>
-      <c r="I91" s="17"/>
-      <c r="J91" s="17"/>
+      <c r="I91" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="J91" s="16" t="s">
+        <v>94</v>
+      </c>
       <c r="K91" s="17"/>
       <c r="L91" s="17"/>
       <c r="M91" s="17"/>
@@ -4980,50 +5032,64 @@
       <c r="AB91" s="17"/>
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="17"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-      <c r="G92" s="5"/>
-      <c r="H92" s="5"/>
-      <c r="I92" s="5"/>
-      <c r="J92" s="5"/>
-      <c r="K92" s="5"/>
-      <c r="L92" s="5"/>
-      <c r="M92" s="5"/>
-      <c r="N92" s="5"/>
-      <c r="O92" s="5"/>
-      <c r="P92" s="5"/>
-      <c r="Q92" s="5"/>
-      <c r="R92" s="5"/>
-      <c r="S92" s="5"/>
-      <c r="T92" s="5"/>
-      <c r="U92" s="5"/>
-      <c r="V92" s="5"/>
-      <c r="W92" s="5"/>
-      <c r="X92" s="5"/>
-      <c r="Y92" s="5"/>
-      <c r="Z92" s="5"/>
-      <c r="AA92" s="5"/>
-      <c r="AB92" s="5"/>
+      <c r="A92" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="B92" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C92" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="D92" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="E92" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F92" s="17"/>
+      <c r="G92" s="17"/>
+      <c r="H92" s="17"/>
+      <c r="I92" s="17"/>
+      <c r="J92" s="17"/>
+      <c r="K92" s="17"/>
+      <c r="L92" s="17"/>
+      <c r="M92" s="17"/>
+      <c r="N92" s="17"/>
+      <c r="O92" s="17"/>
+      <c r="P92" s="17"/>
+      <c r="Q92" s="17"/>
+      <c r="R92" s="17"/>
+      <c r="S92" s="17"/>
+      <c r="T92" s="17"/>
+      <c r="U92" s="17"/>
+      <c r="V92" s="17"/>
+      <c r="W92" s="17"/>
+      <c r="X92" s="17"/>
+      <c r="Y92" s="17"/>
+      <c r="Z92" s="17"/>
+      <c r="AA92" s="17"/>
+      <c r="AB92" s="17"/>
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="17" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="B93" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C93" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="D93" s="18"/>
-      <c r="E93" s="17"/>
-      <c r="F93" s="17"/>
+        <v>215</v>
+      </c>
+      <c r="C93" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="D93" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="E93" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F93" s="17" t="s">
+        <v>218</v>
+      </c>
       <c r="G93" s="17"/>
       <c r="H93" s="17"/>
       <c r="I93" s="17"/>
@@ -5049,11 +5115,11 @@
     </row>
     <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
-        <v>26</v>
+        <v>219</v>
       </c>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
+      <c r="D94" s="17"/>
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
       <c r="G94" s="5"/>
@@ -5080,142 +5146,138 @@
       <c r="AB94" s="5"/>
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="5" t="s">
+      <c r="A95" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B95" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="D95" s="18"/>
+      <c r="E95" s="17"/>
+      <c r="F95" s="17"/>
+      <c r="G95" s="17"/>
+      <c r="H95" s="17"/>
+      <c r="I95" s="17"/>
+      <c r="J95" s="17"/>
+      <c r="K95" s="17"/>
+      <c r="L95" s="17"/>
+      <c r="M95" s="17"/>
+      <c r="N95" s="17"/>
+      <c r="O95" s="17"/>
+      <c r="P95" s="17"/>
+      <c r="Q95" s="17"/>
+      <c r="R95" s="17"/>
+      <c r="S95" s="17"/>
+      <c r="T95" s="17"/>
+      <c r="U95" s="17"/>
+      <c r="V95" s="17"/>
+      <c r="W95" s="17"/>
+      <c r="X95" s="17"/>
+      <c r="Y95" s="17"/>
+      <c r="Z95" s="17"/>
+      <c r="AA95" s="17"/>
+      <c r="AB95" s="17"/>
+    </row>
+    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A96" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="5"/>
+      <c r="I96" s="5"/>
+      <c r="J96" s="5"/>
+      <c r="K96" s="5"/>
+      <c r="L96" s="5"/>
+      <c r="M96" s="5"/>
+      <c r="N96" s="5"/>
+      <c r="O96" s="5"/>
+      <c r="P96" s="5"/>
+      <c r="Q96" s="5"/>
+      <c r="R96" s="5"/>
+      <c r="S96" s="5"/>
+      <c r="T96" s="5"/>
+      <c r="U96" s="5"/>
+      <c r="V96" s="5"/>
+      <c r="W96" s="5"/>
+      <c r="X96" s="5"/>
+      <c r="Y96" s="5"/>
+      <c r="Z96" s="5"/>
+      <c r="AA96" s="5"/>
+      <c r="AB96" s="5"/>
+    </row>
+    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A97" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B95" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="C95" s="17" t="s">
+      <c r="B97" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C97" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D95" s="17"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="H95" s="5"/>
-      <c r="I95" s="5"/>
-      <c r="J95" s="5"/>
-      <c r="K95" s="5"/>
-      <c r="L95" s="5"/>
-      <c r="M95" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="N95" s="5"/>
-      <c r="O95" s="5"/>
-      <c r="P95" s="5"/>
-      <c r="Q95" s="5"/>
-      <c r="R95" s="5"/>
-      <c r="S95" s="5"/>
-      <c r="T95" s="5"/>
-      <c r="U95" s="5"/>
-      <c r="V95" s="5"/>
-      <c r="W95" s="5"/>
-      <c r="X95" s="5"/>
-      <c r="Y95" s="5"/>
-      <c r="Z95" s="5"/>
-      <c r="AA95" s="5"/>
-      <c r="AB95" s="5"/>
-    </row>
-    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="B96" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="C96" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D96" s="17"/>
-      <c r="E96" s="17"/>
-      <c r="F96" s="17"/>
-      <c r="G96" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="H96" s="17"/>
-      <c r="I96" s="17"/>
-      <c r="J96" s="17"/>
-      <c r="K96" s="17"/>
-      <c r="L96" s="17"/>
-      <c r="M96" s="17"/>
-      <c r="N96" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="O96" s="17"/>
-      <c r="P96" s="17"/>
-      <c r="Q96" s="17"/>
-      <c r="R96" s="17"/>
-      <c r="S96" s="17"/>
-      <c r="T96" s="17"/>
-      <c r="U96" s="17"/>
-      <c r="V96" s="17"/>
-      <c r="W96" s="17"/>
-      <c r="X96" s="17"/>
-      <c r="Y96" s="17"/>
-      <c r="Z96" s="17"/>
-      <c r="AA96" s="17"/>
-      <c r="AB96" s="17"/>
-    </row>
-    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B97" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C97" s="17"/>
       <c r="D97" s="17"/>
-      <c r="E97" s="17"/>
-      <c r="F97" s="17"/>
-      <c r="G97" s="17"/>
-      <c r="H97" s="17"/>
-      <c r="I97" s="17"/>
-      <c r="J97" s="17"/>
-      <c r="K97" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="L97" s="17"/>
-      <c r="M97" s="17"/>
-      <c r="N97" s="17"/>
-      <c r="O97" s="17"/>
-      <c r="P97" s="17"/>
-      <c r="Q97" s="17"/>
-      <c r="R97" s="17"/>
-      <c r="S97" s="17"/>
-      <c r="T97" s="17"/>
-      <c r="U97" s="17"/>
-      <c r="V97" s="17"/>
-      <c r="W97" s="17"/>
-      <c r="X97" s="17"/>
-      <c r="Y97" s="17"/>
-      <c r="Z97" s="17"/>
-      <c r="AA97" s="17"/>
-      <c r="AB97" s="17"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="H97" s="5"/>
+      <c r="I97" s="5"/>
+      <c r="J97" s="5"/>
+      <c r="K97" s="5"/>
+      <c r="L97" s="5"/>
+      <c r="M97" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="N97" s="5"/>
+      <c r="O97" s="5"/>
+      <c r="P97" s="5"/>
+      <c r="Q97" s="5"/>
+      <c r="R97" s="5"/>
+      <c r="S97" s="5"/>
+      <c r="T97" s="5"/>
+      <c r="U97" s="5"/>
+      <c r="V97" s="5"/>
+      <c r="W97" s="5"/>
+      <c r="X97" s="5"/>
+      <c r="Y97" s="5"/>
+      <c r="Z97" s="5"/>
+      <c r="AA97" s="5"/>
+      <c r="AB97" s="5"/>
     </row>
     <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="17" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="B98" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="C98" s="17"/>
+        <v>133</v>
+      </c>
+      <c r="C98" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="D98" s="17"/>
       <c r="E98" s="17"/>
       <c r="F98" s="17"/>
-      <c r="G98" s="17"/>
+      <c r="G98" s="17" t="s">
+        <v>132</v>
+      </c>
       <c r="H98" s="17"/>
       <c r="I98" s="17"/>
       <c r="J98" s="17"/>
-      <c r="K98" s="17" t="s">
-        <v>169</v>
-      </c>
+      <c r="K98" s="17"/>
       <c r="L98" s="17"/>
       <c r="M98" s="17"/>
-      <c r="N98" s="17"/>
+      <c r="N98" s="17" t="s">
+        <v>134</v>
+      </c>
       <c r="O98" s="17"/>
       <c r="P98" s="17"/>
       <c r="Q98" s="17"/>
@@ -5236,7 +5298,7 @@
         <v>85</v>
       </c>
       <c r="B99" s="17" t="s">
-        <v>227</v>
+        <v>1</v>
       </c>
       <c r="C99" s="17"/>
       <c r="D99" s="17"/>
@@ -5247,7 +5309,7 @@
       <c r="I99" s="17"/>
       <c r="J99" s="17"/>
       <c r="K99" s="17" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="L99" s="17"/>
       <c r="M99" s="17"/>
@@ -5269,10 +5331,10 @@
     </row>
     <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="17" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="B100" s="17" t="s">
-        <v>28</v>
+        <v>224</v>
       </c>
       <c r="C100" s="17"/>
       <c r="D100" s="17"/>
@@ -5283,12 +5345,10 @@
       <c r="I100" s="17"/>
       <c r="J100" s="17"/>
       <c r="K100" s="17" t="s">
-        <v>229</v>
+        <v>175</v>
       </c>
       <c r="L100" s="17"/>
-      <c r="M100" s="17" t="s">
-        <v>167</v>
-      </c>
+      <c r="M100" s="17"/>
       <c r="N100" s="17"/>
       <c r="O100" s="17"/>
       <c r="P100" s="17"/>
@@ -5305,65 +5365,107 @@
       <c r="AA100" s="17"/>
       <c r="AB100" s="17"/>
     </row>
-    <row r="102" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+    <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A101" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B101" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="C101" s="17"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="17"/>
+      <c r="F101" s="17"/>
+      <c r="G101" s="17"/>
+      <c r="H101" s="17"/>
+      <c r="I101" s="17"/>
+      <c r="J101" s="17"/>
+      <c r="K101" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="L101" s="17"/>
+      <c r="M101" s="17"/>
+      <c r="N101" s="17"/>
+      <c r="O101" s="17"/>
+      <c r="P101" s="17"/>
+      <c r="Q101" s="17"/>
+      <c r="R101" s="17"/>
+      <c r="S101" s="17"/>
+      <c r="T101" s="17"/>
+      <c r="U101" s="17"/>
+      <c r="V101" s="17"/>
+      <c r="W101" s="17"/>
+      <c r="X101" s="17"/>
+      <c r="Y101" s="17"/>
+      <c r="Z101" s="17"/>
+      <c r="AA101" s="17"/>
+      <c r="AB101" s="17"/>
+    </row>
+    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B102" s="0" t="s">
+      <c r="B102" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
+      <c r="F102" s="17"/>
+      <c r="G102" s="17"/>
+      <c r="H102" s="17"/>
+      <c r="I102" s="17"/>
+      <c r="J102" s="17"/>
+      <c r="K102" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="L102" s="17"/>
+      <c r="M102" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="N102" s="17"/>
+      <c r="O102" s="17"/>
+      <c r="P102" s="17"/>
+      <c r="Q102" s="17"/>
+      <c r="R102" s="17"/>
+      <c r="S102" s="17"/>
+      <c r="T102" s="17"/>
+      <c r="U102" s="17"/>
+      <c r="V102" s="17"/>
+      <c r="W102" s="17"/>
+      <c r="X102" s="17"/>
+      <c r="Y102" s="17"/>
+      <c r="Z102" s="17"/>
+      <c r="AA102" s="17"/>
+      <c r="AB102" s="17"/>
+    </row>
+    <row r="104" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="C104" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="G104" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="C102" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="G102" s="0" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B103" s="17" t="s">
-        <v>233</v>
-      </c>
-      <c r="C103" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="D103" s="17"/>
-      <c r="G103" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="H103" s="17"/>
-    </row>
-    <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B104" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="C104" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="D104" s="17"/>
-      <c r="G104" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="H104" s="17"/>
     </row>
     <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B105" s="17" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C105" s="17" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="D105" s="17"/>
       <c r="G105" s="17" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H105" s="17"/>
     </row>
@@ -5372,79 +5474,236 @@
         <v>37</v>
       </c>
       <c r="B106" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="C106" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="D106" s="17"/>
+      <c r="G106" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="H106" s="17"/>
+    </row>
+    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A107" s="17"/>
+      <c r="B107" s="17"/>
+      <c r="C107" s="17"/>
+      <c r="D107" s="17"/>
+      <c r="G107" s="17"/>
+      <c r="H107" s="17"/>
+    </row>
+    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A108" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B108" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="C108" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="D108" s="17"/>
+      <c r="G108" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="H108" s="17"/>
+    </row>
+    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A109" s="17"/>
+      <c r="B109" s="17"/>
+      <c r="C109" s="23"/>
+      <c r="D109" s="17"/>
+      <c r="F109" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="G109" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="H109" s="17"/>
+    </row>
+    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A110" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B110" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="C110" s="23" t="s">
         <v>240</v>
       </c>
-      <c r="C106" s="17" t="s">
+      <c r="D110" s="17"/>
+      <c r="F110" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="D106" s="17"/>
-    </row>
-    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="5" t="s">
+      <c r="G110" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="H110" s="17"/>
+    </row>
+    <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A111" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B111" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="C111" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="D111" s="17"/>
+      <c r="F111" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="G111" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="H111" s="17"/>
+    </row>
+    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A112" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B112" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="C112" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="D112" s="17"/>
+      <c r="F112" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="G112" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="H112" s="17"/>
+    </row>
+    <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A113" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B113" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="C113" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="D113" s="17"/>
+      <c r="F113" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="G113" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="H113" s="17"/>
+    </row>
+    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A114" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B114" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="C114" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="D114" s="17"/>
+      <c r="F114" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="G114" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="H114" s="17"/>
+    </row>
+    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A115" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B115" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="C115" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="D115" s="17"/>
+      <c r="F115" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G115" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="H115" s="17"/>
+    </row>
+    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A116" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B116" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="C116" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="D116" s="17"/>
+    </row>
+    <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A117" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B107" s="5"/>
-      <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
-      <c r="E107" s="5"/>
-      <c r="F107" s="5"/>
-      <c r="G107" s="5"/>
-      <c r="H107" s="5"/>
-      <c r="I107" s="5"/>
-      <c r="J107" s="5"/>
-      <c r="K107" s="5"/>
-      <c r="L107" s="5"/>
-      <c r="M107" s="5"/>
-      <c r="N107" s="5"/>
-      <c r="O107" s="5"/>
-      <c r="P107" s="5"/>
-      <c r="Q107" s="5"/>
-      <c r="R107" s="5"/>
-      <c r="S107" s="5"/>
-      <c r="T107" s="5"/>
-      <c r="U107" s="5"/>
-      <c r="V107" s="5"/>
-      <c r="W107" s="5"/>
-      <c r="X107" s="5"/>
-      <c r="Y107" s="5"/>
-      <c r="Z107" s="5"/>
-      <c r="AA107" s="5"/>
-      <c r="AB107" s="5"/>
-    </row>
-    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B117" s="5"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
+      <c r="F117" s="5"/>
+      <c r="G117" s="5"/>
+      <c r="H117" s="5"/>
+      <c r="I117" s="5"/>
+      <c r="J117" s="5"/>
+      <c r="K117" s="5"/>
+      <c r="L117" s="5"/>
+      <c r="M117" s="5"/>
+      <c r="N117" s="5"/>
+      <c r="O117" s="5"/>
+      <c r="P117" s="5"/>
+      <c r="Q117" s="5"/>
+      <c r="R117" s="5"/>
+      <c r="S117" s="5"/>
+      <c r="T117" s="5"/>
+      <c r="U117" s="5"/>
+      <c r="V117" s="5"/>
+      <c r="W117" s="5"/>
+      <c r="X117" s="5"/>
+      <c r="Y117" s="5"/>
+      <c r="Z117" s="5"/>
+      <c r="AA117" s="5"/>
+      <c r="AB117" s="5"/>
+    </row>
     <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6298,12 +6557,16 @@
     <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1002" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1003" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -6322,11 +6585,11 @@
   </sheetPr>
   <dimension ref="A1:W1014"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10"/>
@@ -6337,14 +6600,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
-        <v>242</v>
-      </c>
-      <c r="B1" s="23" t="s">
+      <c r="A1" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>243</v>
+      <c r="C1" s="25" t="s">
+        <v>259</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -6368,14 +6631,14 @@
       <c r="W1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
-        <v>244</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>245</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>246</v>
+      <c r="A2" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>262</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -6399,14 +6662,14 @@
       <c r="W2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
-        <v>244</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>247</v>
+      <c r="A3" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>263</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -6431,13 +6694,13 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -6462,13 +6725,13 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>110</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -6493,13 +6756,13 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -6524,13 +6787,13 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -6554,14 +6817,14 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="25" t="s">
-        <v>256</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>257</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>258</v>
+      <c r="A8" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>273</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>274</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -6585,14 +6848,14 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25" t="s">
-        <v>256</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>259</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>260</v>
+      <c r="A9" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>276</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -6616,14 +6879,14 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25" t="s">
-        <v>261</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>262</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>263</v>
+      <c r="A10" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>278</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>279</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -6647,14 +6910,14 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="25" t="s">
-        <v>261</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>264</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>265</v>
+      <c r="A11" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>281</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -6678,14 +6941,14 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="25" t="s">
-        <v>266</v>
-      </c>
-      <c r="B12" s="25" t="s">
+      <c r="A12" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="B12" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="25" t="s">
-        <v>258</v>
+      <c r="C12" s="27" t="s">
+        <v>274</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -6709,14 +6972,14 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="s">
-        <v>266</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>267</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>260</v>
+      <c r="A13" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>276</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -6740,14 +7003,14 @@
       <c r="W13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="25" t="s">
-        <v>268</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>269</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>270</v>
+      <c r="A14" s="27" t="s">
+        <v>284</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>285</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>286</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -6771,14 +7034,14 @@
       <c r="W14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="25" t="s">
-        <v>268</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>271</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>272</v>
+      <c r="A15" s="27" t="s">
+        <v>284</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>287</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>288</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -6802,14 +7065,14 @@
       <c r="W15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="25" t="s">
-        <v>268</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>273</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>274</v>
+      <c r="A16" s="27" t="s">
+        <v>284</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>290</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -6833,14 +7096,14 @@
       <c r="W16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="25" t="s">
-        <v>268</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>275</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>276</v>
+      <c r="A17" s="27" t="s">
+        <v>284</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>292</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -6864,14 +7127,14 @@
       <c r="W17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="25" t="s">
-        <v>268</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>254</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>255</v>
+      <c r="A18" s="27" t="s">
+        <v>284</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>270</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>271</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -6895,14 +7158,14 @@
       <c r="W18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26" t="s">
-        <v>277</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>278</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>279</v>
+      <c r="A19" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>295</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -6926,14 +7189,14 @@
       <c r="W19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="26" t="s">
-        <v>277</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>280</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>281</v>
+      <c r="A20" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>297</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -6957,14 +7220,14 @@
       <c r="W20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="26" t="s">
-        <v>277</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>282</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>283</v>
+      <c r="A21" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>298</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>299</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -6988,14 +7251,14 @@
       <c r="W21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>285</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>286</v>
+      <c r="A22" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>301</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>302</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -7019,14 +7282,14 @@
       <c r="W22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="B23" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>287</v>
+      <c r="A23" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>303</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -7050,14 +7313,14 @@
       <c r="W23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>288</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>289</v>
+      <c r="A24" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>305</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -7081,14 +7344,14 @@
       <c r="W24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="B25" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>291</v>
+      <c r="A25" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>306</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>307</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -7112,14 +7375,14 @@
       <c r="W25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>293</v>
+      <c r="A26" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>308</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>309</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -7143,14 +7406,14 @@
       <c r="W26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="B27" s="27" t="s">
-        <v>254</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>255</v>
+      <c r="A27" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>271</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -7174,102 +7437,102 @@
       <c r="W27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>311</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="27" t="s">
+        <v>322</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="27" t="s">
+        <v>322</v>
+      </c>
+      <c r="B35" s="31" t="s">
         <v>294</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="C35" s="30" t="s">
         <v>295</v>
       </c>
-      <c r="C28" s="28" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="25" t="s">
-        <v>294</v>
-      </c>
-      <c r="B29" s="27" t="s">
-        <v>296</v>
-      </c>
-      <c r="C29" s="28" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="25" t="s">
-        <v>294</v>
-      </c>
-      <c r="B30" s="27" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="27" t="s">
+        <v>322</v>
+      </c>
+      <c r="B36" s="31" t="s">
         <v>298</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C36" s="30" t="s">
         <v>299</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="25" t="s">
-        <v>294</v>
-      </c>
-      <c r="B31" s="27" t="s">
-        <v>300</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="B32" s="29" t="s">
-        <v>302</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>304</v>
-      </c>
-      <c r="C33" s="28" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>280</v>
-      </c>
-      <c r="C34" s="28" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="B35" s="29" t="s">
-        <v>278</v>
-      </c>
-      <c r="C35" s="28" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="B36" s="29" t="s">
-        <v>282</v>
-      </c>
-      <c r="C36" s="28" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -8272,7 +8535,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.71"/>
@@ -8287,19 +8550,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>307</v>
+        <v>323</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>308</v>
+        <v>324</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>309</v>
+        <v>325</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>310</v>
+        <v>326</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="2"/>
@@ -8324,19 +8587,19 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>311</v>
+        <v>327</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>313</v>
+        <v>328</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>329</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>314</v>
+        <v>330</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>315</v>
+        <v>331</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -9361,7 +9624,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="1.86"/>
@@ -9374,18 +9637,18 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="31" t="s">
-        <v>316</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
-        <v>317</v>
-      </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31" t="s">
-        <v>318</v>
-      </c>
-      <c r="F1" s="31"/>
+      <c r="A1" s="33" t="s">
+        <v>332</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="F1" s="33"/>
       <c r="G1" s="17"/>
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
@@ -9435,7 +9698,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>319</v>
+        <v>335</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="5"/>
@@ -9464,10 +9727,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>320</v>
+        <v>336</v>
       </c>
       <c r="B4" s="17"/>
-      <c r="C4" s="32"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
@@ -9493,10 +9756,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>321</v>
+        <v>337</v>
       </c>
       <c r="B5" s="17"/>
-      <c r="C5" s="33"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
@@ -9522,10 +9785,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>322</v>
+        <v>338</v>
       </c>
       <c r="B6" s="17"/>
-      <c r="C6" s="34"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
@@ -9551,10 +9814,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>323</v>
+        <v>339</v>
       </c>
       <c r="B7" s="17"/>
-      <c r="C7" s="35"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>

</xml_diff>